<commit_message>
demo pva with\ notes
</commit_message>
<xml_diff>
--- a/static/schedule.xlsx
+++ b/static/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna\Desktop\projects\ssa-200\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876514A0-5D55-41AE-9451-938257F74A55}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45B7E0D-3921-4B6C-B3BD-1DC99EEB6394}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8424" xr2:uid="{97D70F69-AB00-4F24-81FE-0B1143C66DBF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="25">
   <si>
     <t>topic</t>
   </si>
@@ -460,7 +460,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,7 +579,7 @@
         <v>1335</v>
       </c>
       <c r="C10">
-        <v>1345</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -589,6 +589,12 @@
       <c r="B11">
         <v>1420</v>
       </c>
+      <c r="C11">
+        <v>1430</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -597,6 +603,9 @@
       <c r="B12">
         <v>1445</v>
       </c>
+      <c r="C12">
+        <v>1445</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -605,6 +614,9 @@
       <c r="B13">
         <v>1600</v>
       </c>
+      <c r="C13">
+        <v>1600</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -613,24 +625,33 @@
       <c r="B14">
         <v>1700</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
       <c r="B17">
         <v>800</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
       <c r="B18">
         <v>825</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -638,7 +659,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -646,7 +667,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -654,7 +675,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -662,7 +683,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -670,7 +691,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -678,7 +699,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -686,7 +707,7 @@
         <v>1340</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -694,7 +715,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -702,7 +723,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -710,7 +731,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>13</v>
       </c>

</xml_diff>